<commit_message>
removed old backup, replaced switch with jumper
</commit_message>
<xml_diff>
--- a/pcb/kicad/export/bottom/po_midi_adapter.xlsx
+++ b/pcb/kicad/export/bottom/po_midi_adapter.xlsx
@@ -1,12 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="po_midi_adapter" sheetId="1" r:id="rId4"/>
+    <sheet name="po_midi_adapter" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -64,7 +68,7 @@
     <t>LED_SMD:LED_0805_2012Metric_Pad1.15x1.40mm_HandSolder</t>
   </si>
   <si>
-    <t>C401117</t>
+    <t>C409784</t>
   </si>
   <si>
     <t>R10</t>
@@ -143,16 +147,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -161,35 +174,139 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment/>
     </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
+      <alignment/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,20 +504,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{afdf1f20-1463-47ae-b232-8e2a2ac95fb3}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.634285714285713" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="52.88"/>
-    <col customWidth="1" min="4" max="4" width="40.13"/>
+    <col min="3" max="3" width="52.857142857142854" customWidth="1"/>
+    <col min="4" max="4" width="40.142857142857146" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -428,7 +548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -442,7 +562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -456,7 +576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -470,9 +590,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="1">
-        <v>68.0</v>
+        <v>68</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
@@ -484,7 +604,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -498,7 +618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" ht="15.75">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -512,7 +632,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" ht="15.75">
       <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
@@ -526,7 +646,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" ht="15.75">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -540,7 +660,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" ht="15.75">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -554,7 +674,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" ht="15.75">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -569,6 +689,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>